<commit_message>
Added confidence intervals and fixed typos
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg2359\Google Drive (sg2359@cornell.edu)\Projects\CausalInference\table3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg2359\Google Drive (sg2359@cornell.edu)\Projects\CausalInference\table3\mutualfundindia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,6 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="temp" localSheetId="2">Sheet3!$C$7:$E$15</definedName>
+    <definedName name="temp" localSheetId="8">Sheet9!$D$31:$J$49</definedName>
     <definedName name="temp_1" localSheetId="2">Sheet3!$C$19:$E$27</definedName>
     <definedName name="temp_1" localSheetId="7">Sheet8!$E$15:$I$33</definedName>
   </definedNames>
@@ -77,11 +78,24 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="temp3" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\sg2359\Desktop\temp.txt" delimited="0">
+      <textFields count="7">
+        <textField/>
+        <textField position="23"/>
+        <textField position="32"/>
+        <textField position="42"/>
+        <textField position="54"/>
+        <textField position="65"/>
+        <textField position="75"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>Year</t>
   </si>
@@ -315,6 +329,9 @@
   </si>
   <si>
     <t>Coefficients</t>
+  </si>
+  <si>
+    <t>stddev</t>
   </si>
 </sst>
 </file>
@@ -371,13 +388,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,6 +540,108 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet9!$I$14:$I$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>-0.379</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-0.45479999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.6149</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-0.45419999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-0.41739999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.3742999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.40710000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.4345</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.61060000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.42270000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.63349999999999995</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet9!$H$14:$H$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>-1.4936</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>-1.5672999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-0.39929999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-1.5145999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>-1.5308999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.54700000000000004</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>-1.2699999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>-0.35389999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>-7.4899999999999994E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>-0.15160000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>-0.68710000000000004</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:strRef>
               <c:f>Sheet9!$F$14:$F$24</c:f>
@@ -1364,16 +1483,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1405,6 +1524,10 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="temp" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1686,18 +1809,18 @@
   </cols>
   <sheetData>
     <row r="5" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2120,18 +2243,18 @@
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2633,10 +2756,10 @@
       <c r="G20">
         <v>7.0639000000000003</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="Q20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R20" s="6"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -2956,32 +3079,32 @@
   </cols>
   <sheetData>
     <row r="13" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
+      <c r="I14" s="7"/>
+      <c r="J14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
@@ -3102,18 +3225,18 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="5:12" x14ac:dyDescent="0.25">
@@ -3398,7 +3521,7 @@
         <v>0.35606054545454546</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" ref="G17:L17" si="0">AVERAGE(G6:G16)</f>
+        <f t="shared" ref="G17:K17" si="0">AVERAGE(G6:G16)</f>
         <v>1.7601010000000001</v>
       </c>
       <c r="H17" s="4">
@@ -3448,20 +3571,20 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="7" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="3:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3469,374 +3592,374 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>0.1154</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
     </row>
     <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>-5.9400000000000001E-2</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>0.47</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
     </row>
     <row r="22" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <v>0.1943</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>0.71340000000000003</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-    </row>
-    <row r="25" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="3:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>-0.3679</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="7">
+    <row r="26" spans="3:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="5">
         <v>0.40799999999999997</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3881,12 +4004,12 @@
   </cols>
   <sheetData>
     <row r="13" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
@@ -4236,108 +4359,654 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F14:G24"/>
+  <dimension ref="D13:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="10" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>63</v>
       </c>
       <c r="G14">
         <v>-0.93630000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>-1.4936</v>
+      </c>
+      <c r="I14">
+        <v>-0.379</v>
+      </c>
+      <c r="J14">
+        <v>0.2828</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>64</v>
       </c>
       <c r="G15">
         <v>-1.0111000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>-1.5672999999999999</v>
+      </c>
+      <c r="I15">
+        <v>-0.45479999999999998</v>
+      </c>
+      <c r="J15">
+        <v>0.28220000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>65</v>
       </c>
       <c r="G16">
         <v>0.10780000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>-0.39929999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.6149</v>
+      </c>
+      <c r="J16">
+        <v>0.25729999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>66</v>
       </c>
       <c r="G17">
         <v>-0.98440000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>-1.5145999999999999</v>
+      </c>
+      <c r="I17">
+        <v>-0.45419999999999999</v>
+      </c>
+      <c r="J17">
+        <v>0.26900000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>67</v>
       </c>
       <c r="G18">
         <v>-0.97409999999999997</v>
       </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>-1.5308999999999999</v>
+      </c>
+      <c r="I18">
+        <v>-0.41739999999999999</v>
+      </c>
+      <c r="J18">
+        <v>0.28249999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>21</v>
       </c>
       <c r="G19">
         <v>1.9605999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="I19">
+        <v>3.3742999999999999</v>
+      </c>
+      <c r="J19">
+        <v>0.71730000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>68</v>
       </c>
       <c r="G20">
         <v>0.19719999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>-1.2699999999999999E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.40710000000000002</v>
+      </c>
+      <c r="J20">
+        <v>0.1065</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>69</v>
       </c>
       <c r="G21">
         <v>4.0300000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>-0.35389999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.4345</v>
+      </c>
+      <c r="J21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>70</v>
       </c>
       <c r="G22">
         <v>0.26779999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>-7.4899999999999994E-2</v>
+      </c>
+      <c r="I22">
+        <v>0.61060000000000003</v>
+      </c>
+      <c r="J22">
+        <v>0.1739</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>71</v>
       </c>
       <c r="G23">
         <v>0.13550000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>-0.15160000000000001</v>
+      </c>
+      <c r="I23">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="J23">
+        <v>0.1457</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>72</v>
       </c>
       <c r="G24">
         <v>-2.6800000000000001E-2</v>
       </c>
+      <c r="H24">
+        <v>-0.68710000000000004</v>
+      </c>
+      <c r="I24">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="J24">
+        <v>0.33510000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>0.76149999999999995</v>
+      </c>
+      <c r="F31">
+        <v>0.27729999999999999</v>
+      </c>
+      <c r="G31">
+        <v>2.7463000000000002</v>
+      </c>
+      <c r="H31">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="I31">
+        <v>0.215</v>
+      </c>
+      <c r="J31">
+        <v>1.3079000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F32">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G32">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H32">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I32">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="J32">
+        <v>4.2700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>-0.35639999999999999</v>
+      </c>
+      <c r="F33">
+        <v>1.7185999999999999</v>
+      </c>
+      <c r="G33">
+        <v>-0.2074</v>
+      </c>
+      <c r="H33">
+        <v>0.83589999999999998</v>
+      </c>
+      <c r="I33">
+        <v>-3.7433000000000001</v>
+      </c>
+      <c r="J33">
+        <v>3.0305</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34">
+        <v>-0.91200000000000003</v>
+      </c>
+      <c r="F34">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="G34">
+        <v>-1.3441000000000001</v>
+      </c>
+      <c r="H34">
+        <v>0.18029999999999999</v>
+      </c>
+      <c r="I34">
+        <v>-2.2492000000000001</v>
+      </c>
+      <c r="J34">
+        <v>0.42520000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35">
+        <v>-1.3369</v>
+      </c>
+      <c r="F35">
+        <v>0.65</v>
+      </c>
+      <c r="G35">
+        <v>-2.0566</v>
+      </c>
+      <c r="H35">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="I35">
+        <v>-2.6179000000000001</v>
+      </c>
+      <c r="J35">
+        <v>-5.5800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36">
+        <v>-1.6829000000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="G36">
+        <v>-2.2959999999999998</v>
+      </c>
+      <c r="H36">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="I36">
+        <v>-3.1274000000000002</v>
+      </c>
+      <c r="J36">
+        <v>-0.2384</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>-1.7334000000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.21590000000000001</v>
+      </c>
+      <c r="G37">
+        <v>-8.0268999999999995</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>-2.1589</v>
+      </c>
+      <c r="J37">
+        <v>-1.3078000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38">
+        <v>1.9605999999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.71730000000000005</v>
+      </c>
+      <c r="G38">
+        <v>2.7332999999999998</v>
+      </c>
+      <c r="H38">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="I38">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="J38">
+        <v>3.3742999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39">
+        <v>-0.44729999999999998</v>
+      </c>
+      <c r="F39">
+        <v>0.4098</v>
+      </c>
+      <c r="G39">
+        <v>-1.0914999999999999</v>
+      </c>
+      <c r="H39">
+        <v>0.2762</v>
+      </c>
+      <c r="I39">
+        <v>-1.2551000000000001</v>
+      </c>
+      <c r="J39">
+        <v>0.3604</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40">
+        <v>-0.93630000000000002</v>
+      </c>
+      <c r="F40">
+        <v>0.2828</v>
+      </c>
+      <c r="G40">
+        <v>-3.3111999999999999</v>
+      </c>
+      <c r="H40">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="I40">
+        <v>-1.4936</v>
+      </c>
+      <c r="J40">
+        <v>-0.379</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41">
+        <v>-1.0111000000000001</v>
+      </c>
+      <c r="F41">
+        <v>0.28220000000000001</v>
+      </c>
+      <c r="G41">
+        <v>-3.5823</v>
+      </c>
+      <c r="H41">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I41">
+        <v>-1.5672999999999999</v>
+      </c>
+      <c r="J41">
+        <v>-0.45479999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="F42">
+        <v>0.25729999999999997</v>
+      </c>
+      <c r="G42">
+        <v>0.41889999999999999</v>
+      </c>
+      <c r="H42">
+        <v>0.67569999999999997</v>
+      </c>
+      <c r="I42">
+        <v>-0.39929999999999999</v>
+      </c>
+      <c r="J42">
+        <v>0.6149</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43">
+        <v>-0.98440000000000005</v>
+      </c>
+      <c r="F43">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G43">
+        <v>-3.6589</v>
+      </c>
+      <c r="H43">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I43">
+        <v>-1.5145999999999999</v>
+      </c>
+      <c r="J43">
+        <v>-0.45419999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44">
+        <v>-0.97409999999999997</v>
+      </c>
+      <c r="F44">
+        <v>0.28249999999999997</v>
+      </c>
+      <c r="G44">
+        <v>-3.4481000000000002</v>
+      </c>
+      <c r="H44">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I44">
+        <v>-1.5308999999999999</v>
+      </c>
+      <c r="J44">
+        <v>-0.41739999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45">
+        <v>0.19719999999999999</v>
+      </c>
+      <c r="F45">
+        <v>0.1065</v>
+      </c>
+      <c r="G45">
+        <v>1.8520000000000001</v>
+      </c>
+      <c r="H45">
+        <v>6.54E-2</v>
+      </c>
+      <c r="I45">
+        <v>-1.2699999999999999E-2</v>
+      </c>
+      <c r="J45">
+        <v>0.40710000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="F46">
+        <v>0.2</v>
+      </c>
+      <c r="G46">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="H46">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="I46">
+        <v>-0.35389999999999999</v>
+      </c>
+      <c r="J46">
+        <v>0.4345</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47">
+        <v>0.26779999999999998</v>
+      </c>
+      <c r="F47">
+        <v>0.1739</v>
+      </c>
+      <c r="G47">
+        <v>1.5399</v>
+      </c>
+      <c r="H47">
+        <v>0.125</v>
+      </c>
+      <c r="I47">
+        <v>-7.4899999999999994E-2</v>
+      </c>
+      <c r="J47">
+        <v>0.61060000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="F48">
+        <v>0.1457</v>
+      </c>
+      <c r="G48">
+        <v>0.93020000000000003</v>
+      </c>
+      <c r="H48">
+        <v>0.3533</v>
+      </c>
+      <c r="I48">
+        <v>-0.15160000000000001</v>
+      </c>
+      <c r="J48">
+        <v>0.42270000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49">
+        <v>-2.6800000000000001E-2</v>
+      </c>
+      <c r="F49">
+        <v>0.33510000000000001</v>
+      </c>
+      <c r="G49">
+        <v>-8.0100000000000005E-2</v>
+      </c>
+      <c r="H49">
+        <v>0.93620000000000003</v>
+      </c>
+      <c r="I49">
+        <v>-0.68710000000000004</v>
+      </c>
+      <c r="J49">
+        <v>0.63349999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>